<commit_message>
perbaikan log dan capture result
</commit_message>
<xml_diff>
--- a/Data Files/LisSkenarioBaru.xlsx
+++ b/Data Files/LisSkenarioBaru.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Katalon\ASIC\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C2A0EC-E53D-434D-B314-64188334D2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6FEC04-CCD9-4DB1-9462-EC47354D5311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="793" activeTab="2" xr2:uid="{757C07E9-73FD-4EAE-8969-0533CFDE11EA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="793" activeTab="5" xr2:uid="{757C07E9-73FD-4EAE-8969-0533CFDE11EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Batch" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="378">
   <si>
     <t>NoTC</t>
   </si>
@@ -1905,7 +1905,7 @@
   <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5754,8 +5754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70752A91-83F7-4766-8B3A-6B1F070C7186}">
   <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7:P7"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6339,25 +6339,35 @@
         <v>0</v>
       </c>
       <c r="G7" s="4">
-        <v>19784</v>
+        <v>76331</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>52</v>
       </c>
       <c r="I7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="4">
+        <v>19784</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="P7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
@@ -8468,8 +8478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7F4889-46AF-4808-B06F-ACED5C6C53AF}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
menambah gitignore lis skenario
</commit_message>
<xml_diff>
--- a/Data Files/LisSkenarioBaru.xlsx
+++ b/Data Files/LisSkenarioBaru.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Katalon\ASIC\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6FEC04-CCD9-4DB1-9462-EC47354D5311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475044D7-57F3-4766-9872-08E1BC47EFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="793" activeTab="5" xr2:uid="{757C07E9-73FD-4EAE-8969-0533CFDE11EA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="793" activeTab="1" xr2:uid="{757C07E9-73FD-4EAE-8969-0533CFDE11EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Batch" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="374">
   <si>
     <t>NoTC</t>
   </si>
@@ -1150,63 +1150,6 @@
     <t>isBucket</t>
   </si>
   <si>
-    <t>A7241</t>
-  </si>
-  <si>
-    <t>A7242</t>
-  </si>
-  <si>
-    <t>A7243</t>
-  </si>
-  <si>
-    <t>A7244</t>
-  </si>
-  <si>
-    <t>A7245</t>
-  </si>
-  <si>
-    <t>A7246</t>
-  </si>
-  <si>
-    <t>A7247</t>
-  </si>
-  <si>
-    <t>A7248</t>
-  </si>
-  <si>
-    <t>A7249</t>
-  </si>
-  <si>
-    <t>A7250</t>
-  </si>
-  <si>
-    <t>A7251</t>
-  </si>
-  <si>
-    <t>A7252</t>
-  </si>
-  <si>
-    <t>A7253</t>
-  </si>
-  <si>
-    <t>A7254</t>
-  </si>
-  <si>
-    <t>A7255</t>
-  </si>
-  <si>
-    <t>A7256</t>
-  </si>
-  <si>
-    <t>A7257</t>
-  </si>
-  <si>
-    <t>A7258</t>
-  </si>
-  <si>
-    <t>A7259</t>
-  </si>
-  <si>
     <t>col2</t>
   </si>
   <si>
@@ -1226,6 +1169,51 @@
   </si>
   <si>
     <t>A802</t>
+  </si>
+  <si>
+    <t>TC-01</t>
+  </si>
+  <si>
+    <t>TC-02</t>
+  </si>
+  <si>
+    <t>TC-03</t>
+  </si>
+  <si>
+    <t>TC-04</t>
+  </si>
+  <si>
+    <t>TC-05</t>
+  </si>
+  <si>
+    <t>TC-06</t>
+  </si>
+  <si>
+    <t>TC-07</t>
+  </si>
+  <si>
+    <t>TC-08</t>
+  </si>
+  <si>
+    <t>TC-09</t>
+  </si>
+  <si>
+    <t>TC-10</t>
+  </si>
+  <si>
+    <t>TC-11</t>
+  </si>
+  <si>
+    <t>TC-12</t>
+  </si>
+  <si>
+    <t>TC-13</t>
+  </si>
+  <si>
+    <t>TC-14</t>
+  </si>
+  <si>
+    <t>TC-15</t>
   </si>
 </sst>
 </file>
@@ -1905,7 +1893,7 @@
   <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1972,11 +1960,11 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="B2" s="7" t="str">
-        <f t="shared" ref="B2:B18" si="0">CONCATENATE(A2,"-","01")</f>
-        <v>A7241-01</v>
+        <f>CONCATENATE(A2,)</f>
+        <v>TC-01</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="7" t="s">
@@ -2009,16 +1997,16 @@
       <c r="M2" s="7"/>
       <c r="N2" s="20">
         <f>IF(A2&lt;&gt;"",COUNTIF(Activity!A:A,A2),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="B3" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>A7242-01</v>
+        <f t="shared" ref="B3:B22" si="0">CONCATENATE(A3,)</f>
+        <v>TC-02</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="7" t="s">
@@ -2051,16 +2039,16 @@
       <c r="M3" s="7"/>
       <c r="N3" s="20">
         <f>IF(A3&lt;&gt;"",COUNTIF(Activity!A:A,A3),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="B4" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A7243-01</v>
+        <v>TC-03</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="7" t="s">
@@ -2093,16 +2081,16 @@
       <c r="M4" s="7"/>
       <c r="N4" s="20">
         <f>IF(A4&lt;&gt;"",COUNTIF(Activity!A:A,A4),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="B5" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A7244-01</v>
+        <v>TC-04</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="7" t="s">
@@ -2135,16 +2123,16 @@
       <c r="M5" s="7"/>
       <c r="N5" s="20">
         <f>IF(A5&lt;&gt;"",COUNTIF(Activity!A:A,A5),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="B6" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A7245-01</v>
+        <v>TC-05</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="7" t="s">
@@ -2177,16 +2165,16 @@
       <c r="M6" s="7"/>
       <c r="N6" s="20">
         <f>IF(A6&lt;&gt;"",COUNTIF(Activity!A:A,A6),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="B7" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A7246-01</v>
+        <v>TC-06</v>
       </c>
       <c r="C7" s="30"/>
       <c r="D7" s="7" t="s">
@@ -2219,16 +2207,16 @@
       <c r="M7" s="7"/>
       <c r="N7" s="20">
         <f>IF(A7&lt;&gt;"",COUNTIF(Activity!A:A,A7),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="B8" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A7247-01</v>
+        <v>TC-07</v>
       </c>
       <c r="C8" s="30"/>
       <c r="D8" s="7" t="s">
@@ -2261,16 +2249,16 @@
       <c r="M8" s="7"/>
       <c r="N8" s="20">
         <f>IF(A8&lt;&gt;"",COUNTIF(Activity!A:A,A8),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="B9" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A7248-01</v>
+        <v>TC-08</v>
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="7" t="s">
@@ -2303,16 +2291,16 @@
       <c r="M9" s="7"/>
       <c r="N9" s="20">
         <f>IF(A9&lt;&gt;"",COUNTIF(Activity!A:A,A9),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="B10" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A7249-01</v>
+        <v>TC-09</v>
       </c>
       <c r="C10" s="30"/>
       <c r="D10" s="7" t="s">
@@ -2345,16 +2333,16 @@
       <c r="M10" s="7"/>
       <c r="N10" s="20">
         <f>IF(A10&lt;&gt;"",COUNTIF(Activity!A:A,A10),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="B11" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A7250-01</v>
+        <v>TC-10</v>
       </c>
       <c r="C11" s="30"/>
       <c r="D11" s="7" t="s">
@@ -2387,16 +2375,16 @@
       <c r="M11" s="7"/>
       <c r="N11" s="20">
         <f>IF(A11&lt;&gt;"",COUNTIF(Activity!A:A,A11),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="B12" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A7251-01</v>
+        <v>TC-11</v>
       </c>
       <c r="C12" s="30"/>
       <c r="D12" s="7" t="s">
@@ -2429,16 +2417,16 @@
       <c r="M12" s="7"/>
       <c r="N12" s="20">
         <f>IF(A12&lt;&gt;"",COUNTIF(Activity!A:A,A12),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="B13" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A7252-01</v>
+        <v>TC-12</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="7" t="s">
@@ -2471,16 +2459,16 @@
       <c r="M13" s="7"/>
       <c r="N13" s="20">
         <f>IF(A13&lt;&gt;"",COUNTIF(Activity!A:A,A13),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="B14" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A7253-01</v>
+        <v>TC-13</v>
       </c>
       <c r="C14" s="30"/>
       <c r="D14" s="7" t="s">
@@ -2513,16 +2501,16 @@
       <c r="M14" s="7"/>
       <c r="N14" s="20">
         <f>IF(A14&lt;&gt;"",COUNTIF(Activity!A:A,A14),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="B15" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A7254-01</v>
+        <v>TC-14</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="7" t="s">
@@ -2555,16 +2543,16 @@
       <c r="M15" s="7"/>
       <c r="N15" s="20">
         <f>IF(A15&lt;&gt;"",COUNTIF(Activity!A:A,A15),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="B16" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A7255-01</v>
+        <v>TC-15</v>
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="7" t="s">
@@ -2597,16 +2585,14 @@
       <c r="M16" s="7"/>
       <c r="N16" s="20">
         <f>IF(A16&lt;&gt;"",COUNTIF(Activity!A:A,A16),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="27" t="s">
-        <v>367</v>
-      </c>
+      <c r="A17" s="27"/>
       <c r="B17" s="7" t="str">
-        <f>CONCATENATE(A17,"-","01")</f>
-        <v>A7256-01</v>
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="C17" s="30"/>
       <c r="D17" s="7" t="s">
@@ -2637,18 +2623,16 @@
         <v>187</v>
       </c>
       <c r="M17" s="7"/>
-      <c r="N17" s="20">
+      <c r="N17" s="20" t="str">
         <f>IF(A17&lt;&gt;"",COUNTIF(Activity!A:A,A17),"")</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="27" t="s">
-        <v>368</v>
-      </c>
+      <c r="A18" s="27"/>
       <c r="B18" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A7257-01</v>
+        <v/>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="7" t="s">
@@ -2679,18 +2663,16 @@
         <v>187</v>
       </c>
       <c r="M18" s="7"/>
-      <c r="N18" s="20">
+      <c r="N18" s="20" t="str">
         <f>IF(A18&lt;&gt;"",COUNTIF(Activity!A:A,A18),"")</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="27" t="s">
-        <v>369</v>
-      </c>
+      <c r="A19" s="27"/>
       <c r="B19" s="7" t="str">
-        <f t="shared" ref="B19" si="1">CONCATENATE(A19,"-","01")</f>
-        <v>A7258-01</v>
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="C19" s="30"/>
       <c r="D19" s="7" t="s">
@@ -2721,18 +2703,16 @@
         <v>187</v>
       </c>
       <c r="M19" s="7"/>
-      <c r="N19" s="20">
+      <c r="N19" s="20" t="str">
         <f>IF(A19&lt;&gt;"",COUNTIF(Activity!A:A,A19),"")</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="27" t="s">
-        <v>370</v>
-      </c>
+      <c r="A20" s="27"/>
       <c r="B20" s="7" t="str">
-        <f t="shared" ref="B20:B22" si="2">CONCATENATE(A20,"-","01")</f>
-        <v>A7259-01</v>
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="C20" s="30"/>
       <c r="D20" s="7" t="s">
@@ -2763,25 +2743,23 @@
         <v>187</v>
       </c>
       <c r="M20" s="7"/>
-      <c r="N20" s="20">
+      <c r="N20" s="20" t="str">
         <f>IF(A20&lt;&gt;"",COUNTIF(Activity!A:A,A20),"")</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="27" t="s">
-        <v>373</v>
-      </c>
+      <c r="A21" s="27"/>
       <c r="B21" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>A801-01</v>
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>374</v>
+        <v>355</v>
       </c>
       <c r="F21" s="7">
         <v>11353</v>
@@ -2805,18 +2783,16 @@
         <v>187</v>
       </c>
       <c r="M21" s="7"/>
-      <c r="N21" s="20">
+      <c r="N21" s="20" t="str">
         <f>IF(A21&lt;&gt;"",COUNTIF(Activity!A:A,A21),"")</f>
-        <v>19</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="29" t="s">
-        <v>377</v>
-      </c>
+      <c r="A22" s="29"/>
       <c r="B22" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>A802-01</v>
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="C22" s="30" t="s">
         <v>300</v>
@@ -2849,9 +2825,9 @@
         <v>187</v>
       </c>
       <c r="M22" s="7"/>
-      <c r="N22" s="20">
+      <c r="N22" s="20" t="str">
         <f>IF(A22&lt;&gt;"",COUNTIF(Activity!A:A,A22),"")</f>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -5223,8 +5199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D923057-5622-4B75-B52E-77EA52D2CA36}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5267,11 +5243,11 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="B2" s="3" t="str">
         <f>IF(A2="", "",VLOOKUP(A2,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>Bucket Rek COLL = 1, Kode Restruk Blank</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -5290,11 +5266,11 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="B3" s="3" t="str">
         <f>IF(A3="", "",VLOOKUP(A3,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>Bucket Rek COLL = 2, Kode Restruk Blank</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
@@ -5313,11 +5289,11 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="B4" s="3" t="str">
         <f>IF(A4="", "",VLOOKUP(A4,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>Bucket Rek COLL = 1, Kode Restruk 8</v>
       </c>
       <c r="C4" s="3">
         <v>3</v>
@@ -5336,11 +5312,11 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="B5" s="3" t="str">
         <f>IF(A5="", "",VLOOKUP(A5,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>Bucket Rek COLL = 2, Kode Restruk 8</v>
       </c>
       <c r="C5" s="3">
         <v>4</v>
@@ -5359,11 +5335,11 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="B6" s="3" t="str">
         <f>IF(A6="", "",VLOOKUP(A6,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>Bucket Rek COLL = 1, Kode Restruk Selain Blank dan 8</v>
       </c>
       <c r="C6" s="3">
         <v>5</v>
@@ -5382,11 +5358,11 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="B7" s="3" t="str">
         <f>IF(A7="", "",VLOOKUP(A7,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>Bucket Rek COLL = 2, Kode Restruk Selain Blank dan 8</v>
       </c>
       <c r="C7" s="3">
         <v>6</v>
@@ -5405,11 +5381,11 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="B8" s="3" t="str">
         <f>IF(A8="", "",VLOOKUP(A8,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>Bucket Rek COLL = 3, Kode Restruk Blank</v>
       </c>
       <c r="C8" s="3">
         <v>7</v>
@@ -5428,11 +5404,11 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="B9" s="3" t="str">
         <f>IF(A9="", "",VLOOKUP(A9,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>Bucket Rek COLL = 4, Kode Restruk Blank</v>
       </c>
       <c r="C9" s="3">
         <v>8</v>
@@ -5451,11 +5427,11 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="B10" s="3" t="str">
         <f>IF(A10="", "",VLOOKUP(A10,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>Bucket Rek COLL = 5, Kode Restruk Blank</v>
       </c>
       <c r="C10" s="3">
         <v>9</v>
@@ -5474,11 +5450,11 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B11" s="3" t="str">
         <f>IF(A11="", "",VLOOKUP(A11,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>Bucket Rek COLL = 3, Kode Restruk 8</v>
       </c>
       <c r="C11" s="3">
         <v>10</v>
@@ -5497,11 +5473,11 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B12" s="3" t="str">
         <f>IF(A12="", "",VLOOKUP(A12,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>Bucket Rek COLL = 4, Kode Restruk 8</v>
       </c>
       <c r="C12" s="3">
         <v>11</v>
@@ -5520,11 +5496,11 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B13" s="3" t="str">
         <f>IF(A13="", "",VLOOKUP(A13,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>Bucket Rek COLL = 5, Kode Restruk 8</v>
       </c>
       <c r="C13" s="3">
         <v>12</v>
@@ -5543,11 +5519,11 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B14" s="3" t="str">
         <f>IF(A14="", "",VLOOKUP(A14,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>Bucket Rek COLL = 3, Kode Restruk Selain Blank dan 8</v>
       </c>
       <c r="C14" s="3">
         <v>13</v>
@@ -5566,11 +5542,11 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B15" s="3" t="str">
         <f>IF(A15="", "",VLOOKUP(A15,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>Bucket Rek COLL = 4, Kode Restruk Selain Blank dan 8</v>
       </c>
       <c r="C15" s="3">
         <v>14</v>
@@ -5593,7 +5569,7 @@
       </c>
       <c r="B16" s="3" t="str">
         <f>IF(A16="", "",VLOOKUP(A16,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>Bucket Rek COLL = 5, Kode Restruk Selain Blank dan 8</v>
       </c>
       <c r="C16" s="3">
         <v>15</v>
@@ -5612,11 +5588,11 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
-        <v>373</v>
-      </c>
-      <c r="B17" s="3" t="str">
+        <v>354</v>
+      </c>
+      <c r="B17" s="3" t="e">
         <f>IF(A17="", "",VLOOKUP(A17,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>#N/A</v>
       </c>
       <c r="C17" s="3">
         <v>16</v>
@@ -5635,11 +5611,11 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
-        <v>373</v>
-      </c>
-      <c r="B18" s="3" t="str">
+        <v>354</v>
+      </c>
+      <c r="B18" s="3" t="e">
         <f>IF(A18="", "",VLOOKUP(A18,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>#N/A</v>
       </c>
       <c r="C18" s="3">
         <v>17</v>
@@ -5658,11 +5634,11 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
-        <v>373</v>
-      </c>
-      <c r="B19" s="3" t="str">
+        <v>354</v>
+      </c>
+      <c r="B19" s="3" t="e">
         <f>IF(A19="", "",VLOOKUP(A19,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>#N/A</v>
       </c>
       <c r="C19" s="3">
         <v>18</v>
@@ -5681,11 +5657,11 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>373</v>
-      </c>
-      <c r="B20" s="3" t="str">
+        <v>354</v>
+      </c>
+      <c r="B20" s="3" t="e">
         <f>IF(A20="", "",VLOOKUP(A20,Batch!A:E,5,FALSE))</f>
-        <v>Retest Bucket, Asuransi, Pinbuk</v>
+        <v>#N/A</v>
       </c>
       <c r="C20" s="3">
         <v>19</v>
@@ -5704,11 +5680,11 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
-        <v>377</v>
-      </c>
-      <c r="B21" s="3" t="str">
+        <v>358</v>
+      </c>
+      <c r="B21" s="3" t="e">
         <f>IF(A21="", "",VLOOKUP(A21,Batch!A:E,5,FALSE))</f>
-        <v>Rekening WORST COLLECTIBILITY = 1, Kode Restruk Selain Blank dan 8</v>
+        <v>#N/A</v>
       </c>
       <c r="C21" s="3">
         <v>1</v>
@@ -8478,8 +8454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7F4889-46AF-4808-B06F-ACED5C6C53AF}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8554,7 +8530,7 @@
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="str" cm="1">
         <f t="array" ref="A3:A18">_xlfn._xlws.FILTER(Activity!A:A,(Activity!A:A&lt;&gt;"")*(Activity!D:D=A1)*(Activity!C:C&lt;&gt;"""")*(Activity!G:G&lt;&gt;"Y"))</f>
-        <v>A801</v>
+        <v>TC-01</v>
       </c>
       <c r="B3" s="3" cm="1">
         <f t="array" ref="B3:D18">_xlfn._xlws.FILTER(Activity!C:E,(Activity!A:A&lt;&gt;"")*(Activity!D:D=A1)*(Activity!G:G&lt;&gt;"Y"))</f>
@@ -8600,7 +8576,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="str">
-        <v>A801</v>
+        <v>TC-02</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
@@ -8645,7 +8621,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="str">
-        <v>A801</v>
+        <v>TC-03</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
@@ -8690,7 +8666,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="str">
-        <v>A801</v>
+        <v>TC-04</v>
       </c>
       <c r="B6" s="3">
         <v>4</v>
@@ -8735,7 +8711,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="str">
-        <v>A801</v>
+        <v>TC-05</v>
       </c>
       <c r="B7" s="3">
         <v>5</v>
@@ -8780,7 +8756,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="str">
-        <v>A801</v>
+        <v>TC-06</v>
       </c>
       <c r="B8" s="3">
         <v>6</v>
@@ -8825,7 +8801,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="str">
-        <v>A801</v>
+        <v>TC-07</v>
       </c>
       <c r="B9" s="3">
         <v>7</v>
@@ -8870,7 +8846,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="str">
-        <v>A801</v>
+        <v>TC-08</v>
       </c>
       <c r="B10" s="3">
         <v>8</v>
@@ -8915,7 +8891,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="str">
-        <v>A801</v>
+        <v>TC-09</v>
       </c>
       <c r="B11" s="3">
         <v>9</v>
@@ -8960,7 +8936,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="str">
-        <v>A801</v>
+        <v>TC-10</v>
       </c>
       <c r="B12" s="3">
         <v>10</v>
@@ -9005,7 +8981,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="str">
-        <v>A801</v>
+        <v>TC-11</v>
       </c>
       <c r="B13" s="3">
         <v>11</v>
@@ -9050,7 +9026,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="str">
-        <v>A801</v>
+        <v>TC-12</v>
       </c>
       <c r="B14" s="3">
         <v>12</v>
@@ -9095,7 +9071,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="str">
-        <v>A801</v>
+        <v>TC-13</v>
       </c>
       <c r="B15" s="3">
         <v>13</v>
@@ -9140,7 +9116,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="str">
-        <v>A801</v>
+        <v>TC-14</v>
       </c>
       <c r="B16" s="3">
         <v>14</v>
@@ -9185,7 +9161,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="str">
-        <v>A801</v>
+        <v>TC-15</v>
       </c>
       <c r="B17" s="3">
         <v>15</v>
@@ -9628,13 +9604,13 @@
         <v>10000</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>372</v>
+        <v>353</v>
       </c>
       <c r="M3" s="14">
         <v>228356776</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>375</v>
+        <v>356</v>
       </c>
       <c r="O3" s="16" t="s">
         <v>167</v>
@@ -9684,13 +9660,13 @@
         <v>10000</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>371</v>
+        <v>352</v>
       </c>
       <c r="M4" s="14">
         <v>228356776</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>376</v>
+        <v>357</v>
       </c>
       <c r="O4" s="16" t="s">
         <v>167</v>

</xml_diff>